<commit_message>
Arreglado ejemplo cercha real, añadidos comentarios
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\PycharmProjects\CalculadoraCerchasExcel\discretizacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2024-a\ConvertirPt\CalculadoraCerchasExcel\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B906A9-9D8A-4ACE-AFD3-D70924A20235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06609E02-69AA-4900-9B81-EDED0623A2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nodos" sheetId="1" r:id="rId1"/>
-    <sheet name="Elementos" sheetId="3" r:id="rId2"/>
+    <sheet name="Elementos" sheetId="3" r:id="rId1"/>
+    <sheet name="Nodos" sheetId="1" r:id="rId2"/>
     <sheet name="Datos" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t>X</t>
   </si>
@@ -127,10 +127,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,11 +463,268 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7662DF1-C715-49DB-B57A-AA4CA6C1A83B}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0AEB2F-FBF5-4B25-A985-03D41A1E807E}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,13 +769,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
@@ -527,19 +783,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>2</v>
+        <v>-100</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -553,135 +809,262 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-100</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-100</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>12</v>
       </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7662DF1-C715-49DB-B57A-AA4CA6C1A83B}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-100</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-100</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-100</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -694,18 +1077,18 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Añadidas las subrutinas para calcular el nband y de pin_jointed
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2024-a\ConvertirPt\CalculadoraCerchasExcel\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\PycharmProjects\CalculadoraCerchasExcel\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1157EA89-8396-4D34-9124-198DF49CE7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE590CE-5BA7-45D1-A3F9-12678E394843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Elementos" sheetId="3" r:id="rId1"/>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7662DF1-C715-49DB-B57A-AA4CA6C1A83B}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +562,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1">
         <v>5</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1">
         <v>5</v>
@@ -650,7 +650,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1">
         <v>8</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1">
         <v>7</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1">
         <v>7</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1">
         <v>10</v>
@@ -723,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0AEB2F-FBF5-4B25-A985-03D41A1E807E}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +812,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -864,7 +864,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -916,7 +916,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -968,7 +968,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1020,7 +1020,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Datos arreglados y añadido 3 dimensiones, arreglada la subrutina pin_jointed
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\PycharmProjects\CalculadoraCerchasExcel\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE590CE-5BA7-45D1-A3F9-12678E394843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06AD23C-F00F-4009-B0B3-98D34AED269C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Elementos" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>X</t>
   </si>
@@ -55,9 +55,6 @@
     <t>FY</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>DIM</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
   </si>
   <si>
     <t>Rest_z</t>
+  </si>
+  <si>
+    <t>FZ</t>
   </si>
 </sst>
 </file>
@@ -127,9 +127,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7662DF1-C715-49DB-B57A-AA4CA6C1A83B}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -474,13 +475,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -721,15 +722,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0AEB2F-FBF5-4B25-A985-03D41A1E807E}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -745,25 +746,28 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+      <c r="C2" s="1">
+        <v>0</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -771,25 +775,28 @@
       <c r="E2" s="1">
         <v>-100</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
+      <c r="C3" s="1">
+        <v>1</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -797,25 +804,28 @@
       <c r="E3" s="1">
         <v>-100</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
+      <c r="F3" s="2">
+        <v>0</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
+      <c r="C4" s="1">
+        <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -823,25 +833,28 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="1">
-        <v>1</v>
+      <c r="F4" s="2">
+        <v>0</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
+      <c r="C5" s="1">
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -849,25 +862,28 @@
       <c r="E5" s="1">
         <v>-100</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
+      <c r="F5" s="2">
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
+      <c r="C6" s="1">
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -875,25 +891,28 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
+      <c r="F6" s="2">
+        <v>0</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
+      <c r="C7" s="1">
+        <v>1</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -901,25 +920,28 @@
       <c r="E7" s="1">
         <v>-100</v>
       </c>
-      <c r="F7" s="1">
-        <v>1</v>
+      <c r="F7" s="2">
+        <v>0</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
+      <c r="C8" s="1">
+        <v>1</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -927,25 +949,28 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
+      <c r="F8" s="2">
+        <v>0</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>12</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
+      <c r="C9" s="1">
+        <v>1</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -953,25 +978,28 @@
       <c r="E9" s="1">
         <v>-100</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
+      <c r="F9" s="2">
+        <v>0</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
+      <c r="C10" s="1">
+        <v>1</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -979,25 +1007,28 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="1">
-        <v>1</v>
+      <c r="F10" s="2">
+        <v>0</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
+      <c r="C11" s="1">
+        <v>1</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -1005,25 +1036,28 @@
       <c r="E11" s="1">
         <v>-100</v>
       </c>
-      <c r="F11" s="1">
-        <v>1</v>
+      <c r="F11" s="2">
+        <v>0</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>15</v>
       </c>
       <c r="B12" s="1">
         <v>4</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
+      <c r="C12" s="1">
+        <v>1</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -1031,25 +1065,28 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
-        <v>1</v>
+      <c r="F12" s="2">
+        <v>0</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>18</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>5</v>
+      <c r="C13" s="1">
+        <v>1</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -1057,14 +1094,17 @@
       <c r="E13" s="1">
         <v>-100</v>
       </c>
-      <c r="F13" s="1">
-        <v>1</v>
+      <c r="F13" s="2">
+        <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1076,15 +1116,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E1F06C-A87F-45D7-8D75-0575F1BF82DF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Datos arreglados y añadidos subrutina form_kv
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\PycharmProjects\CalculadoraCerchasExcel\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06AD23C-F00F-4009-B0B3-98D34AED269C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5D6137-0453-4724-B5EC-1FC9FE46570C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Elementos" sheetId="3" r:id="rId1"/>
@@ -127,10 +127,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7662DF1-C715-49DB-B57A-AA4CA6C1A83B}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +491,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -511,10 +510,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -522,10 +521,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -544,10 +543,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -555,15 +554,15 @@
         <v>1</v>
       </c>
       <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
         <v>3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -574,7 +573,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -585,7 +584,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
@@ -596,24 +595,24 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
         <v>5</v>
-      </c>
-      <c r="C12" s="1">
-        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,10 +631,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -651,7 +650,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1">
         <v>8</v>
@@ -662,7 +661,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="1">
         <v>7</v>
@@ -673,7 +672,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="1">
         <v>7</v>
@@ -684,7 +683,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="1">
         <v>10</v>
@@ -698,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1">
         <v>11</v>
@@ -709,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1">
         <v>11</v>
@@ -725,7 +724,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +745,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -775,7 +774,7 @@
       <c r="E2" s="1">
         <v>-100</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>0</v>
       </c>
       <c r="G2" s="1">
@@ -804,7 +803,7 @@
       <c r="E3" s="1">
         <v>-100</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>0</v>
       </c>
       <c r="G3" s="1">
@@ -833,7 +832,7 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" s="1">
@@ -862,7 +861,7 @@
       <c r="E5" s="1">
         <v>-100</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>0</v>
       </c>
       <c r="G5" s="1">
@@ -891,7 +890,7 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>0</v>
       </c>
       <c r="G6" s="1">
@@ -920,7 +919,7 @@
       <c r="E7" s="1">
         <v>-100</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>0</v>
       </c>
       <c r="G7" s="1">
@@ -949,7 +948,7 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>0</v>
       </c>
       <c r="G8" s="1">
@@ -978,7 +977,7 @@
       <c r="E9" s="1">
         <v>-100</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="G9" s="1">
@@ -1007,7 +1006,7 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>0</v>
       </c>
       <c r="G10" s="1">
@@ -1036,7 +1035,7 @@
       <c r="E11" s="1">
         <v>-100</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>0</v>
       </c>
       <c r="G11" s="1">
@@ -1065,7 +1064,7 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>0</v>
       </c>
       <c r="G12" s="1">
@@ -1094,7 +1093,7 @@
       <c r="E13" s="1">
         <v>-100</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>0</v>
       </c>
       <c r="G13" s="1">
@@ -1116,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E1F06C-A87F-45D7-8D75-0575F1BF82DF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix props, EA, KV
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\PycharmProjects\CalculadoraCerchasExcel\datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2024-a\ConvertirPt\CalculadoraCerchasExcel\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5D6137-0453-4724-B5EC-1FC9FE46570C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796BA248-0207-40D0-B460-089484F3F5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="11010" windowHeight="12885" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Elementos" sheetId="3" r:id="rId1"/>
     <sheet name="Nodos" sheetId="1" r:id="rId2"/>
     <sheet name="Datos" sheetId="2" r:id="rId3"/>
+    <sheet name="Props" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>X</t>
   </si>
@@ -467,7 +468,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,7 +1117,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,4 +1135,48 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ADB904-29E7-468C-9044-A9315EE87C4A}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5875.2749999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Arreglado banred y bacsub para 1D
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2024-a\ConvertirPt\CalculadoraCerchasExcel\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF131EFB-568E-4BAC-9DEE-FE63B3884FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BFED67-C005-46D2-8140-CCBD7895BB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="3" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Elementos" sheetId="3" r:id="rId1"/>
@@ -128,9 +128,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +469,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +493,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -500,10 +501,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,206 +515,98 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1">
-        <v>6</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1">
-        <v>6</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>5</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1">
-        <v>5</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1">
-        <v>8</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1">
-        <v>7</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1">
-        <v>7</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1">
-        <v>7</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1">
-        <v>10</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1">
-        <v>10</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1">
-        <v>9</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1">
-        <v>10</v>
-      </c>
-      <c r="C20" s="1">
-        <v>9</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1">
-        <v>10</v>
-      </c>
-      <c r="C21" s="1">
-        <v>11</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1">
-        <v>9</v>
-      </c>
-      <c r="C22" s="1">
-        <v>11</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -724,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0AEB2F-FBF5-4B25-A985-03D41A1E807E}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,10 +653,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="1">
@@ -773,12 +666,12 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>-46</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" s="1">
@@ -789,323 +682,179 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>-92</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>-92</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
       <c r="H5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-92</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>-92</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1">
-        <v>1</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1">
-        <v>1</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>15</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>-92</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1">
-        <v>1</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>18</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>-46</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1117,7 +866,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,7 +878,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1141,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ADB904-29E7-468C-9044-A9315EE87C4A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>5875.2749999999996</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1165,7 +914,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>200</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1173,7 +922,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>300</v>
+        <v>840000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix de banred en 1D y 2D
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2024-a\ConvertirPt\CalculadoraCerchasExcel\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF131EFB-568E-4BAC-9DEE-FE63B3884FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA6CE93-6375-4914-9300-70B989D94BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
@@ -725,7 +725,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Incluido deformacion unitaria y esfuerzo
</commit_message>
<xml_diff>
--- a/datos/datos.xlsx
+++ b/datos/datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2024-a\ConvertirPt\CalculadoraCerchasExcel\datos\1d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean7\Documents\2024-a\ConvertirPt\CalculadoraCerchasExcel\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6927CFE1-8FBD-4620-88F5-5AABCFB9320F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0292B97-77C2-4D7E-BD36-E15FBF4F0395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="3" xr2:uid="{7E256D8D-9C75-477B-8580-A8B7BA1AF2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Elementos" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>DIM</t>
   </si>
@@ -80,22 +80,25 @@
     <t>FZ [kN]</t>
   </si>
   <si>
-    <t>Nodo Restringido</t>
-  </si>
-  <si>
-    <t>Nodo Libre</t>
+    <t>A en cm^2</t>
   </si>
   <si>
     <t>Agregar el valor de dimensión (1, 2 o 3)</t>
   </si>
   <si>
-    <t>A en cm^2</t>
-  </si>
-  <si>
     <t>E en GPA (kN/mm^2)</t>
   </si>
   <si>
     <t>AE en 10⁵N (100 kN).</t>
+  </si>
+  <si>
+    <t>Restringido</t>
+  </si>
+  <si>
+    <t>Libre</t>
+  </si>
+  <si>
+    <t>A(cm^2)</t>
   </si>
 </sst>
 </file>
@@ -146,13 +149,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -491,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7662DF1-C715-49DB-B57A-AA4CA6C1A83B}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -524,10 +533,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -538,98 +547,206 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -638,15 +755,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0AEB2F-FBF5-4B25-A985-03D41A1E807E}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -674,12 +791,25 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
+      <c r="K1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="2">
+        <v>0</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2" s="1">
@@ -689,12 +819,12 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>-46</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>0</v>
       </c>
       <c r="H2" s="1">
@@ -703,200 +833,333 @@
       <c r="I2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>-92</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>1</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-92</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-92</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-92</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-92</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-46</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -904,27 +1167,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E1F06C-A87F-45D7-8D75-0575F1BF82DF}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -934,50 +1195,62 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ADB904-29E7-468C-9044-A9315EE87C4A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>840000</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5875.2749999999996</v>
+      </c>
+      <c r="C2">
+        <v>27.977499999999999</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>840000</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5875.2749999999996</v>
+      </c>
+      <c r="C3">
+        <v>27.977499999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>840000</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
+        <v>5875.2749999999996</v>
+      </c>
+      <c r="C4">
+        <v>27.977499999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>